<commit_message>
Response sizes graphics added
</commit_message>
<xml_diff>
--- a/documentation/src/main/resources/statistics/Response sizes.xlsx
+++ b/documentation/src/main/resources/statistics/Response sizes.xlsx
@@ -16,15 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Runs</t>
+    <t>Simulation runs</t>
   </si>
   <si>
-    <t>Time [ms]</t>
+    <t>Time for marshaling [ms]</t>
   </si>
   <si>
-    <t>Size [MB]</t>
+    <t>Size of XML file [MB]</t>
+  </si>
+  <si>
+    <t>Tree size is 1000</t>
   </si>
 </sst>
 </file>
@@ -49,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -57,12 +60,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -70,6 +101,501 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="bg-BG"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Time for marshaling</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1510</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2514</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3057</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3507</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4591</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5038</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5740</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6073</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6680</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7361</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7727</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8203</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8986</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9519</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9685</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10230</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="86848640"/>
+        <c:axId val="86850176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="86848640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86850176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86850176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86848640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="bg-BG"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Size of XML file</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>364</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>511</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>693</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>729</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="79723904"/>
+        <c:axId val="88200320"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79723904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88200320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88200320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79723904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,247 +883,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
         <v>1000</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="1">
         <v>609</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
         <v>2000</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="1">
         <v>1013</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
         <v>3000</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="1">
         <v>1510</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
         <v>4000</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="1">
         <v>2022</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="1">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
         <v>5000</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="1">
         <v>2514</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="1">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
         <v>6000</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="1">
         <v>3057</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="1">
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
         <v>7000</v>
       </c>
-      <c r="B8">
+      <c r="B9" s="1">
         <v>3507</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="1">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
         <v>8000</v>
       </c>
-      <c r="B9">
+      <c r="B10" s="1">
         <v>4013</v>
       </c>
-      <c r="C9">
+      <c r="C10" s="1">
         <v>292</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
         <v>9000</v>
       </c>
-      <c r="B10">
+      <c r="B11" s="1">
         <v>4591</v>
       </c>
-      <c r="C10">
+      <c r="C11" s="1">
         <v>328</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
         <v>10000</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="1">
         <v>5038</v>
       </c>
-      <c r="C11">
+      <c r="C12" s="1">
         <v>364</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
         <v>11000</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="1">
         <v>5740</v>
       </c>
-      <c r="C12">
+      <c r="C13" s="1">
         <v>401</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
         <v>12000</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="1">
         <v>6073</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="1">
         <v>438</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
         <v>13000</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="1">
         <v>6680</v>
       </c>
-      <c r="C14">
+      <c r="C15" s="1">
         <v>474</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
         <v>14000</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="1">
         <v>7361</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="1">
         <v>511</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
         <v>15000</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="1">
         <v>7727</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="1">
         <v>547</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
         <v>16000</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="1">
         <v>8203</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="1">
         <v>583</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
         <v>17000</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="1">
         <v>8986</v>
       </c>
-      <c r="C18">
+      <c r="C19" s="1">
         <v>620</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
         <v>18000</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="1">
         <v>9519</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="1">
         <v>657</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
         <v>19000</v>
       </c>
-      <c r="B20">
+      <c r="B21" s="1">
         <v>9685</v>
       </c>
-      <c r="C20">
+      <c r="C21" s="1">
         <v>693</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
         <v>20000</v>
       </c>
-      <c r="B21">
+      <c r="B22" s="1">
         <v>10230</v>
       </c>
-      <c r="C21">
+      <c r="C22" s="1">
         <v>729</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Developer's guide added to document
</commit_message>
<xml_diff>
--- a/documentation/src/main/resources/statistics/Response sizes.xlsx
+++ b/documentation/src/main/resources/statistics/Response sizes.xlsx
@@ -213,89 +213,89 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>609</c:v>
+                  <c:v>584</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1013</c:v>
+                  <c:v>964</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1510</c:v>
+                  <c:v>1441</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2022</c:v>
+                  <c:v>1901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2514</c:v>
+                  <c:v>2370</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3057</c:v>
+                  <c:v>2860</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3507</c:v>
+                  <c:v>3309</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4013</c:v>
+                  <c:v>3805</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4591</c:v>
+                  <c:v>4286</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5038</c:v>
+                  <c:v>4730</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5740</c:v>
+                  <c:v>5260</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6073</c:v>
+                  <c:v>5806</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6680</c:v>
+                  <c:v>6261</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7361</c:v>
+                  <c:v>6742</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>7207</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>7727</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>8203</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>8986</c:v>
+                  <c:v>8104</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9519</c:v>
+                  <c:v>8526</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9685</c:v>
+                  <c:v>9096</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10230</c:v>
+                  <c:v>9692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="86848640"/>
-        <c:axId val="86850176"/>
+        <c:axId val="117314688"/>
+        <c:axId val="117316224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86848640"/>
+        <c:axId val="117314688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86850176"/>
+        <c:crossAx val="117316224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86850176"/>
+        <c:axId val="117316224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -303,7 +303,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86848640"/>
+        <c:crossAx val="117314688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -312,7 +312,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -428,89 +428,89 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>109</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>146</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>182</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>219</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>255</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>292</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>328</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>364</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>401</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>438</c:v>
+                  <c:v>289</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>474</c:v>
+                  <c:v>313</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>511</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>547</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>583</c:v>
+                  <c:v>385</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>620</c:v>
+                  <c:v>409</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>657</c:v>
+                  <c:v>433</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>693</c:v>
+                  <c:v>457</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>729</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="79723904"/>
-        <c:axId val="88200320"/>
+        <c:axId val="117344512"/>
+        <c:axId val="117370880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="79723904"/>
+        <c:axId val="117344512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88200320"/>
+        <c:crossAx val="117370880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88200320"/>
+        <c:axId val="117370880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,7 +518,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79723904"/>
+        <c:crossAx val="117344512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -527,7 +527,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -886,7 +886,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -919,10 +919,10 @@
         <v>1000</v>
       </c>
       <c r="B3" s="1">
-        <v>609</v>
+        <v>584</v>
       </c>
       <c r="C3" s="1">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -930,10 +930,10 @@
         <v>2000</v>
       </c>
       <c r="B4" s="1">
-        <v>1013</v>
+        <v>964</v>
       </c>
       <c r="C4" s="1">
-        <v>73</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -941,10 +941,10 @@
         <v>3000</v>
       </c>
       <c r="B5" s="1">
-        <v>1510</v>
+        <v>1441</v>
       </c>
       <c r="C5" s="1">
-        <v>109</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -952,10 +952,10 @@
         <v>4000</v>
       </c>
       <c r="B6" s="1">
-        <v>2022</v>
+        <v>1901</v>
       </c>
       <c r="C6" s="1">
-        <v>146</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -963,10 +963,10 @@
         <v>5000</v>
       </c>
       <c r="B7" s="1">
-        <v>2514</v>
+        <v>2370</v>
       </c>
       <c r="C7" s="1">
-        <v>182</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -974,10 +974,10 @@
         <v>6000</v>
       </c>
       <c r="B8" s="1">
-        <v>3057</v>
+        <v>2860</v>
       </c>
       <c r="C8" s="1">
-        <v>219</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -985,10 +985,10 @@
         <v>7000</v>
       </c>
       <c r="B9" s="1">
-        <v>3507</v>
+        <v>3309</v>
       </c>
       <c r="C9" s="1">
-        <v>255</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -996,10 +996,10 @@
         <v>8000</v>
       </c>
       <c r="B10" s="1">
-        <v>4013</v>
+        <v>3805</v>
       </c>
       <c r="C10" s="1">
-        <v>292</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1007,10 +1007,10 @@
         <v>9000</v>
       </c>
       <c r="B11" s="1">
-        <v>4591</v>
+        <v>4286</v>
       </c>
       <c r="C11" s="1">
-        <v>328</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1018,10 +1018,10 @@
         <v>10000</v>
       </c>
       <c r="B12" s="1">
-        <v>5038</v>
+        <v>4730</v>
       </c>
       <c r="C12" s="1">
-        <v>364</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1029,10 +1029,10 @@
         <v>11000</v>
       </c>
       <c r="B13" s="1">
-        <v>5740</v>
+        <v>5260</v>
       </c>
       <c r="C13" s="1">
-        <v>401</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1040,10 +1040,10 @@
         <v>12000</v>
       </c>
       <c r="B14" s="1">
-        <v>6073</v>
+        <v>5806</v>
       </c>
       <c r="C14" s="1">
-        <v>438</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1051,10 +1051,10 @@
         <v>13000</v>
       </c>
       <c r="B15" s="1">
-        <v>6680</v>
+        <v>6261</v>
       </c>
       <c r="C15" s="1">
-        <v>474</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1062,10 +1062,10 @@
         <v>14000</v>
       </c>
       <c r="B16" s="1">
-        <v>7361</v>
+        <v>6742</v>
       </c>
       <c r="C16" s="1">
-        <v>511</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1073,10 +1073,10 @@
         <v>15000</v>
       </c>
       <c r="B17" s="1">
-        <v>7727</v>
+        <v>7207</v>
       </c>
       <c r="C17" s="1">
-        <v>547</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1084,10 +1084,10 @@
         <v>16000</v>
       </c>
       <c r="B18" s="1">
-        <v>8203</v>
+        <v>7727</v>
       </c>
       <c r="C18" s="1">
-        <v>583</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1095,10 +1095,10 @@
         <v>17000</v>
       </c>
       <c r="B19" s="1">
-        <v>8986</v>
+        <v>8104</v>
       </c>
       <c r="C19" s="1">
-        <v>620</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1106,10 +1106,10 @@
         <v>18000</v>
       </c>
       <c r="B20" s="1">
-        <v>9519</v>
+        <v>8526</v>
       </c>
       <c r="C20" s="1">
-        <v>657</v>
+        <v>433</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1117,10 +1117,10 @@
         <v>19000</v>
       </c>
       <c r="B21" s="1">
-        <v>9685</v>
+        <v>9096</v>
       </c>
       <c r="C21" s="1">
-        <v>693</v>
+        <v>457</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1128,10 +1128,10 @@
         <v>20000</v>
       </c>
       <c r="B22" s="1">
-        <v>10230</v>
+        <v>9692</v>
       </c>
       <c r="C22" s="1">
-        <v>729</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>